<commit_message>
add data cleaning file
</commit_message>
<xml_diff>
--- a/datasets/sanitation.xlsx
+++ b/datasets/sanitation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abu aisha\Documents\fi_swb_analysis\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2804C7E6-B4DE-4241-9C2A-EBAB5BD49771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142413AB-2FDC-42E6-8AB7-13E116273048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E8EE1084-A70B-420C-9A34-D0FDF3584C50}"/>
   </bookViews>
@@ -921,10 +921,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13307D9-9B35-4CD9-9F09-C3658D6A083F}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4057,6 +4059,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C88" s="2">
+        <f>SUM(C2:C87)</f>
+        <v>461</v>
+      </c>
+      <c r="F88" s="2">
+        <f>SUM(F2:F87)</f>
+        <v>23</v>
+      </c>
+      <c r="H88" s="2">
+        <f>SUM(H2:H87)</f>
+        <v>20</v>
+      </c>
+      <c r="J88" s="2">
+        <f>SUM(J2:J87)</f>
+        <v>14</v>
+      </c>
+      <c r="K88" s="2">
+        <f>SUM(K2:K87)</f>
+        <v>32</v>
+      </c>
+      <c r="L88" s="2">
+        <f t="shared" ref="L88:N88" si="0">SUM(L2:L87)</f>
+        <v>282</v>
+      </c>
+      <c r="M88" s="2">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="N88" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>